<commit_message>
Actualizacion avance HU en Cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/FC/Gestion/FC-CP.xlsx
+++ b/Desarrollo/FC/Gestion/FC-CP.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos_5toCiclo\GCS_FC\Desarrollo\FC\Gestion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA733DCA-CD7D-486F-BBCF-1AB701E1C44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="7200" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="CRONOGRAMA" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="ROLES" sheetId="2" r:id="rId5"/>
+    <sheet name="CRONOGRAMA" sheetId="1" r:id="rId1"/>
+    <sheet name="ROLES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhRWy3q40HB67231XrValJaoT813w=="/>
@@ -383,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
@@ -391,21 +400,21 @@
   </numFmts>
   <fonts count="31">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF0779E4"/>
       <name val="Montserrat"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
@@ -413,157 +422,163 @@
       <b/>
       <i/>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFAFDCB"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF060606"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF060606"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF060606"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Montserrat"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Montserrat"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -574,7 +589,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -614,33 +629,43 @@
     </fill>
   </fills>
   <borders count="28">
-    <border/>
     <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -650,6 +675,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -664,6 +690,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -678,6 +705,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -692,6 +720,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -706,17 +735,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -729,6 +748,20 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -743,6 +776,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -755,6 +789,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -766,15 +801,8 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -785,6 +813,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -799,6 +839,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -809,6 +850,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -817,6 +859,9 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -825,9 +870,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -842,6 +889,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -854,17 +902,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -877,28 +915,44 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -913,6 +967,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -923,6 +978,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -934,247 +990,222 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="93">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="4" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="10" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="14" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="15" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="6" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="12" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="15" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="14" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="12" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="13" fillId="5" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="5" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="14" fillId="2" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="2" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="2" fontId="18" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="12" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="5" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="4" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="20" fillId="4" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="9" fontId="18" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="21" fillId="5" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="6" fontId="23" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="2" fontId="24" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="2" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="2" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="22" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="7" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="7" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="25" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="7" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="7" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="4" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="24" fillId="2" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="24" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="9" fontId="22" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="25" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="26" fillId="2" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="23" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="9" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="27" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1364,31 +1395,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.88"/>
-    <col customWidth="1" min="2" max="2" width="57.63"/>
-    <col customWidth="1" min="3" max="3" width="57.5"/>
-    <col customWidth="1" min="4" max="4" width="14.5"/>
-    <col customWidth="1" min="5" max="5" width="64.0"/>
-    <col customWidth="1" min="6" max="7" width="10.38"/>
-    <col customWidth="1" min="8" max="8" width="14.38"/>
-    <col customWidth="1" min="9" max="9" width="10.13"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="71.85546875" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="23.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1398,7 +1433,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1409,12 +1444,12 @@
       <c r="G2" s="6"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1422,7 +1457,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1435,7 +1470,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1448,12 +1483,12 @@
       <c r="G5" s="6"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="12">
-        <v>44692.0</v>
+        <v>44692</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="4"/>
@@ -1461,12 +1496,12 @@
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="15">
-        <v>44777.0</v>
+        <v>44777</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="4"/>
@@ -1474,7 +1509,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -1484,7 +1519,7 @@
       <c r="G8" s="17"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1510,604 +1545,618 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A10" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="30">
-        <v>44694.0</v>
-      </c>
-      <c r="G10" s="30">
-        <v>44700.0</v>
-      </c>
-      <c r="H10" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="I10" s="32" t="s">
+      <c r="F10" s="29">
+        <v>44694</v>
+      </c>
+      <c r="G10" s="29">
+        <v>44700</v>
+      </c>
+      <c r="H10" s="30">
+        <v>1</v>
+      </c>
+      <c r="I10" s="31" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="26" t="s">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A11" s="87"/>
+      <c r="B11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="30">
-        <v>44694.0</v>
-      </c>
-      <c r="G11" s="30">
-        <v>44707.0</v>
-      </c>
-      <c r="H11" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="I11" s="32" t="s">
+      <c r="F11" s="29">
+        <v>44694</v>
+      </c>
+      <c r="G11" s="29">
+        <v>44707</v>
+      </c>
+      <c r="H11" s="30">
+        <v>1</v>
+      </c>
+      <c r="I11" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="36"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A12" s="87"/>
+      <c r="B12" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="30">
-        <v>44694.0</v>
-      </c>
-      <c r="G12" s="30">
-        <v>44707.0</v>
-      </c>
-      <c r="H12" s="38">
-        <v>1.0</v>
-      </c>
-      <c r="J12" s="36"/>
+      <c r="F12" s="29">
+        <v>44694</v>
+      </c>
+      <c r="G12" s="29">
+        <v>44707</v>
+      </c>
+      <c r="H12" s="36">
+        <v>1</v>
+      </c>
+      <c r="I12" s="85"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="39" t="s">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A13" s="87"/>
+      <c r="B13" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="30">
-        <v>44694.0</v>
-      </c>
-      <c r="G13" s="30">
-        <v>44707.0</v>
-      </c>
-      <c r="H13" s="38">
-        <v>1.0</v>
-      </c>
+      <c r="F13" s="29">
+        <v>44694</v>
+      </c>
+      <c r="G13" s="29">
+        <v>44707</v>
+      </c>
+      <c r="H13" s="36">
+        <v>1</v>
+      </c>
+      <c r="I13" s="85"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14">
-      <c r="A14" s="33"/>
-      <c r="B14" s="26" t="s">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A14" s="87"/>
+      <c r="B14" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="30">
-        <v>44701.0</v>
-      </c>
-      <c r="G14" s="30">
-        <v>44707.0</v>
-      </c>
-      <c r="H14" s="31"/>
-      <c r="J14" s="36"/>
+      <c r="F14" s="29">
+        <v>44701</v>
+      </c>
+      <c r="G14" s="29">
+        <v>44707</v>
+      </c>
+      <c r="H14" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="85"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="39" t="s">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A15" s="87"/>
+      <c r="B15" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="30">
-        <v>44708.0</v>
-      </c>
-      <c r="G15" s="30">
-        <v>44714.0</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="J15" s="36"/>
+      <c r="F15" s="29">
+        <v>44708</v>
+      </c>
+      <c r="G15" s="29">
+        <v>44714</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="26" t="s">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A16" s="87"/>
+      <c r="B16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="30">
-        <v>44708.0</v>
-      </c>
-      <c r="G16" s="30">
-        <v>44714.0</v>
-      </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="42" t="s">
+      <c r="F16" s="29">
+        <v>44708</v>
+      </c>
+      <c r="G16" s="29">
+        <v>44714</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="36"/>
+      <c r="J16" s="34"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="33"/>
-      <c r="B17" s="43" t="s">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A17" s="87"/>
+      <c r="B17" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="30">
-        <v>44708.0</v>
-      </c>
-      <c r="G17" s="30">
-        <v>44714.0</v>
-      </c>
-      <c r="H17" s="31"/>
-      <c r="J17" s="36"/>
+      <c r="F17" s="29">
+        <v>44708</v>
+      </c>
+      <c r="G17" s="29">
+        <v>44714</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="34"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="33"/>
-      <c r="B18" s="39" t="s">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A18" s="87"/>
+      <c r="B18" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="30">
-        <v>44715.0</v>
-      </c>
-      <c r="G18" s="30">
-        <v>44721.0</v>
-      </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="32" t="s">
+      <c r="F18" s="29">
+        <v>44715</v>
+      </c>
+      <c r="G18" s="29">
+        <v>44721</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="J18" s="36"/>
+      <c r="J18" s="34"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="39" t="s">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A19" s="87"/>
+      <c r="B19" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="30">
-        <v>44715.0</v>
-      </c>
-      <c r="G19" s="30">
-        <v>44721.0</v>
-      </c>
-      <c r="H19" s="31"/>
-      <c r="J19" s="36"/>
+      <c r="F19" s="29">
+        <v>44715</v>
+      </c>
+      <c r="G19" s="29">
+        <v>44721</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="34"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="45"/>
-      <c r="B20" s="46" t="s">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A20" s="88"/>
+      <c r="B20" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="50">
-        <v>44715.0</v>
-      </c>
-      <c r="G20" s="50">
-        <v>44721.0</v>
-      </c>
-      <c r="H20" s="51"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="52" t="s">
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47">
+        <v>44715</v>
+      </c>
+      <c r="G20" s="47">
+        <v>44721</v>
+      </c>
+      <c r="H20" s="48"/>
+      <c r="I20" s="85"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A21" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="30">
-        <v>44722.0</v>
-      </c>
-      <c r="G21" s="30">
-        <v>44728.0</v>
-      </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="42" t="s">
+      <c r="F21" s="29">
+        <v>44722</v>
+      </c>
+      <c r="G21" s="29">
+        <v>44728</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="36"/>
+      <c r="J21" s="34"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="33"/>
-      <c r="B22" s="53" t="s">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A22" s="87"/>
+      <c r="B22" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="30">
-        <v>44722.0</v>
-      </c>
-      <c r="G22" s="30">
-        <v>44728.0</v>
-      </c>
-      <c r="H22" s="55"/>
-      <c r="J22" s="36"/>
+      <c r="F22" s="29">
+        <v>44722</v>
+      </c>
+      <c r="G22" s="29">
+        <v>44728</v>
+      </c>
+      <c r="H22" s="51"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="34"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="56" t="s">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A23" s="87"/>
+      <c r="B23" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="30">
-        <v>44722.0</v>
-      </c>
-      <c r="G23" s="30">
-        <v>44728.0</v>
-      </c>
-      <c r="H23" s="54"/>
-      <c r="J23" s="36"/>
+      <c r="F23" s="29">
+        <v>44722</v>
+      </c>
+      <c r="G23" s="29">
+        <v>44728</v>
+      </c>
+      <c r="H23" s="50"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="34"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="33"/>
-      <c r="B24" s="39" t="s">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A24" s="87"/>
+      <c r="B24" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="57">
-        <v>44729.0</v>
-      </c>
-      <c r="G24" s="30">
-        <v>44742.0</v>
-      </c>
-      <c r="H24" s="55"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="36"/>
+      <c r="F24" s="53">
+        <v>44729</v>
+      </c>
+      <c r="G24" s="29">
+        <v>44742</v>
+      </c>
+      <c r="H24" s="51"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="33"/>
-      <c r="B25" s="26" t="s">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A25" s="87"/>
+      <c r="B25" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="57">
-        <v>44729.0</v>
-      </c>
-      <c r="G25" s="30">
-        <v>44742.0</v>
-      </c>
-      <c r="H25" s="31"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="36"/>
+      <c r="F25" s="53">
+        <v>44729</v>
+      </c>
+      <c r="G25" s="29">
+        <v>44742</v>
+      </c>
+      <c r="H25" s="30"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="34"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="33"/>
-      <c r="B26" s="39" t="s">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A26" s="87"/>
+      <c r="B26" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="30">
-        <v>44736.0</v>
-      </c>
-      <c r="G26" s="30">
-        <v>44742.0</v>
-      </c>
-      <c r="H26" s="31"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="36"/>
+      <c r="F26" s="29">
+        <v>44736</v>
+      </c>
+      <c r="G26" s="29">
+        <v>44742</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="34"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="46" t="s">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A27" s="88"/>
+      <c r="B27" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="59">
-        <v>44736.0</v>
-      </c>
-      <c r="G27" s="59">
-        <v>44742.0</v>
-      </c>
-      <c r="H27" s="60"/>
-      <c r="I27" s="32"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="61" t="s">
+      <c r="C27" s="54"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="55">
+        <v>44736</v>
+      </c>
+      <c r="G27" s="55">
+        <v>44742</v>
+      </c>
+      <c r="H27" s="56"/>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A28" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="30">
-        <v>44743.0</v>
-      </c>
-      <c r="G28" s="30">
-        <v>44749.0</v>
-      </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="42" t="s">
+      <c r="F28" s="29">
+        <v>44743</v>
+      </c>
+      <c r="G28" s="29">
+        <v>44749</v>
+      </c>
+      <c r="H28" s="30"/>
+      <c r="I28" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="J28" s="36"/>
+      <c r="J28" s="34"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="33"/>
-      <c r="B29" s="63" t="s">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A29" s="87"/>
+      <c r="B29" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="30">
-        <v>44750.0</v>
-      </c>
-      <c r="G29" s="30">
-        <v>44756.0</v>
-      </c>
-      <c r="H29" s="31"/>
-      <c r="I29" s="42" t="s">
+      <c r="F29" s="29">
+        <v>44750</v>
+      </c>
+      <c r="G29" s="29">
+        <v>44756</v>
+      </c>
+      <c r="H29" s="30"/>
+      <c r="I29" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="J29" s="36"/>
+      <c r="J29" s="34"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="33"/>
-      <c r="B30" s="63" t="s">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A30" s="87"/>
+      <c r="B30" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="30">
-        <v>44750.0</v>
-      </c>
-      <c r="G30" s="30">
-        <v>44756.0</v>
-      </c>
-      <c r="H30" s="31"/>
-      <c r="J30" s="36"/>
+      <c r="F30" s="29">
+        <v>44750</v>
+      </c>
+      <c r="G30" s="29">
+        <v>44756</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="34"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="65" t="s">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A31" s="87"/>
+      <c r="B31" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="29" t="s">
+      <c r="E31" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="F31" s="30">
-        <v>44750.0</v>
-      </c>
-      <c r="G31" s="30">
-        <v>44756.0</v>
-      </c>
-      <c r="H31" s="31"/>
-      <c r="J31" s="36"/>
+      <c r="F31" s="29">
+        <v>44750</v>
+      </c>
+      <c r="G31" s="29">
+        <v>44756</v>
+      </c>
+      <c r="H31" s="30"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="34"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="33"/>
-      <c r="B32" s="62" t="s">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A32" s="87"/>
+      <c r="B32" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="30">
-        <v>44757.0</v>
-      </c>
-      <c r="G32" s="30">
-        <v>44756.0</v>
-      </c>
-      <c r="H32" s="31"/>
-      <c r="I32" s="42" t="s">
+      <c r="F32" s="29">
+        <v>44757</v>
+      </c>
+      <c r="G32" s="29">
+        <v>44756</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="J32" s="36"/>
+      <c r="J32" s="34"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="33"/>
-      <c r="B33" s="62" t="s">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A33" s="87"/>
+      <c r="B33" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="30">
-        <v>44757.0</v>
-      </c>
-      <c r="G33" s="30">
-        <v>44756.0</v>
-      </c>
-      <c r="H33" s="31"/>
-      <c r="J33" s="36"/>
+      <c r="F33" s="29">
+        <v>44757</v>
+      </c>
+      <c r="G33" s="29">
+        <v>44756</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="34"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2125,1134 +2174,1136 @@
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="33"/>
-      <c r="B34" s="62" t="s">
+    <row r="34" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A34" s="87"/>
+      <c r="B34" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="30">
-        <v>44757.0</v>
-      </c>
-      <c r="G34" s="30">
-        <v>44763.0</v>
-      </c>
-      <c r="H34" s="31"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="36"/>
+      <c r="F34" s="29">
+        <v>44757</v>
+      </c>
+      <c r="G34" s="29">
+        <v>44763</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="34"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="62" t="s">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A35" s="87"/>
+      <c r="B35" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="30">
-        <v>44764.0</v>
-      </c>
-      <c r="G35" s="30">
-        <v>44770.0</v>
-      </c>
-      <c r="H35" s="31"/>
-      <c r="I35" s="42" t="s">
+      <c r="F35" s="29">
+        <v>44764</v>
+      </c>
+      <c r="G35" s="29">
+        <v>44770</v>
+      </c>
+      <c r="H35" s="30"/>
+      <c r="I35" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="J35" s="36"/>
+      <c r="J35" s="34"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="33"/>
-      <c r="B36" s="62" t="s">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="87"/>
+      <c r="B36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="30">
-        <v>44771.0</v>
-      </c>
-      <c r="G36" s="30">
-        <v>44777.0</v>
-      </c>
-      <c r="H36" s="31"/>
-      <c r="I36" s="42" t="s">
+      <c r="F36" s="29">
+        <v>44771</v>
+      </c>
+      <c r="G36" s="29">
+        <v>44777</v>
+      </c>
+      <c r="H36" s="30"/>
+      <c r="I36" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="J36" s="36"/>
+      <c r="J36" s="34"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="66" t="s">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A37" s="87"/>
+      <c r="B37" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="30">
-        <v>44771.0</v>
-      </c>
-      <c r="G37" s="30">
-        <v>44777.0</v>
-      </c>
-      <c r="H37" s="31"/>
-      <c r="J37" s="36"/>
+      <c r="F37" s="29">
+        <v>44771</v>
+      </c>
+      <c r="G37" s="29">
+        <v>44777</v>
+      </c>
+      <c r="H37" s="30"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="34"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="45"/>
-      <c r="B38" s="68" t="s">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A38" s="88"/>
+      <c r="B38" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="50">
-        <v>44771.0</v>
-      </c>
-      <c r="G38" s="50">
-        <v>44777.0</v>
-      </c>
-      <c r="H38" s="72"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="75"/>
-      <c r="B40" s="75"/>
-      <c r="F40" s="76"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="47">
+        <v>44771</v>
+      </c>
+      <c r="G38" s="47">
+        <v>44777</v>
+      </c>
+      <c r="H38" s="67"/>
+      <c r="I38" s="85"/>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A39" s="68"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A40" s="70"/>
+      <c r="B40" s="70"/>
+      <c r="F40" s="71"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="6:8" ht="15.75" customHeight="1">
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="6:8" ht="15.75" customHeight="1">
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="6:8" ht="15.75" customHeight="1">
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="6:8" ht="15.75" customHeight="1">
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="6:8" ht="15.75" customHeight="1">
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="6:8" ht="15.75" customHeight="1">
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="6:8" ht="15.75" customHeight="1">
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="6:8" ht="15.75" customHeight="1">
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="6:8" ht="15.75" customHeight="1">
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="6:8" ht="15.75" customHeight="1">
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="6:8" ht="15.75" customHeight="1">
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="6:8" ht="15.75" customHeight="1">
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="6:8" ht="15.75" customHeight="1">
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="6:8" ht="15.75" customHeight="1">
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="6:8" ht="15.75" customHeight="1">
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="6:8" ht="15.75" customHeight="1">
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="6:8" ht="15.75" customHeight="1">
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="6:8" ht="15.75" customHeight="1">
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="6:8" ht="15.75" customHeight="1">
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="6:8" ht="15.75" customHeight="1">
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="6:8" ht="15.75" customHeight="1">
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="6:8" ht="15.75" customHeight="1">
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="6:8" ht="15.75" customHeight="1">
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="6:8" ht="15.75" customHeight="1">
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="6:8" ht="15.75" customHeight="1">
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="6:8" ht="15.75" customHeight="1">
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="6:8" ht="15.75" customHeight="1">
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="6:8" ht="15.75" customHeight="1">
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="6:8" ht="15.75" customHeight="1">
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="6:8" ht="15.75" customHeight="1">
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="6:8" ht="15.75" customHeight="1">
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="6:8" ht="15.75" customHeight="1">
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="6:8" ht="15.75" customHeight="1">
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="6:8" ht="15.75" customHeight="1">
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="6:8" ht="15.75" customHeight="1">
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="6:8" ht="15.75" customHeight="1">
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="6:8" ht="15.75" customHeight="1">
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="6:8" ht="15.75" customHeight="1">
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="6:8" ht="15.75" customHeight="1">
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="6:8" ht="15.75" customHeight="1">
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="6:8" ht="15.75" customHeight="1">
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="6:8" ht="15.75" customHeight="1">
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="6:8" ht="15.75" customHeight="1">
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="6:8" ht="15.75" customHeight="1">
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="6:8" ht="15.75" customHeight="1">
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="6:8" ht="15.75" customHeight="1">
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="6:8" ht="15.75" customHeight="1">
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="6:8" ht="15.75" customHeight="1">
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="6:8" ht="15.75" customHeight="1">
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="6:8" ht="15.75" customHeight="1">
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="6:8" ht="15.75" customHeight="1">
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="6:8" ht="15.75" customHeight="1">
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="6:8" ht="15.75" customHeight="1">
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="6:8" ht="15.75" customHeight="1">
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="6:8" ht="15.75" customHeight="1">
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="6:8" ht="15.75" customHeight="1">
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="6:8" ht="15.75" customHeight="1">
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="6:8" ht="15.75" customHeight="1">
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="6:8" ht="15.75" customHeight="1">
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="6:8" ht="15.75" customHeight="1">
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="6:8" ht="15.75" customHeight="1">
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="6:8" ht="15.75" customHeight="1">
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="6:8" ht="15.75" customHeight="1">
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="6:8" ht="15.75" customHeight="1">
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="6:8" ht="15.75" customHeight="1">
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="6:8" ht="15.75" customHeight="1">
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="6:8" ht="15.75" customHeight="1">
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
       <c r="H115" s="7"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="6:8" ht="15.75" customHeight="1">
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
       <c r="H116" s="7"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="6:8" ht="15.75" customHeight="1">
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
       <c r="H117" s="7"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="6:8" ht="15.75" customHeight="1">
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="6:8" ht="15.75" customHeight="1">
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="6:8" ht="15.75" customHeight="1">
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="6:8" ht="15.75" customHeight="1">
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
       <c r="H121" s="7"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="6:8" ht="15.75" customHeight="1">
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
       <c r="H122" s="7"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="6:8" ht="15.75" customHeight="1">
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="6:8" ht="15.75" customHeight="1">
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="6:8" ht="15.75" customHeight="1">
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="6:8" ht="15.75" customHeight="1">
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="6:8" ht="15.75" customHeight="1">
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="6:8" ht="15.75" customHeight="1">
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="6:8" ht="15.75" customHeight="1">
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="6:8" ht="15.75" customHeight="1">
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="6:8" ht="15.75" customHeight="1">
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="6:8" ht="15.75" customHeight="1">
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="6:8" ht="15.75" customHeight="1">
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
       <c r="H133" s="7"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="6:8" ht="15.75" customHeight="1">
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
       <c r="H134" s="7"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="6:8" ht="15.75" customHeight="1">
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
       <c r="H135" s="7"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="6:8" ht="15.75" customHeight="1">
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
       <c r="H136" s="7"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="6:8" ht="15.75" customHeight="1">
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="6:8" ht="15.75" customHeight="1">
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="6:8" ht="15.75" customHeight="1">
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="6:8" ht="15.75" customHeight="1">
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="6:8" ht="15.75" customHeight="1">
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="6:8" ht="15.75" customHeight="1">
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
       <c r="H142" s="7"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="6:8" ht="15.75" customHeight="1">
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="6:8" ht="15.75" customHeight="1">
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
       <c r="H144" s="7"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="6:8" ht="15.75" customHeight="1">
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="6:8" ht="15.75" customHeight="1">
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
       <c r="H146" s="7"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="6:8" ht="15.75" customHeight="1">
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="6:8" ht="15.75" customHeight="1">
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="6:8" ht="15.75" customHeight="1">
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="6:8" ht="15.75" customHeight="1">
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
       <c r="H150" s="7"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="6:8" ht="15.75" customHeight="1">
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="6:8" ht="15.75" customHeight="1">
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
       <c r="H152" s="7"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="6:8" ht="15.75" customHeight="1">
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="6:8" ht="15.75" customHeight="1">
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
       <c r="H154" s="7"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="6:8" ht="15.75" customHeight="1">
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
       <c r="H155" s="7"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="6:8" ht="15.75" customHeight="1">
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
       <c r="H156" s="7"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="6:8" ht="15.75" customHeight="1">
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
       <c r="H157" s="7"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="6:8" ht="15.75" customHeight="1">
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
       <c r="H158" s="7"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="6:8" ht="15.75" customHeight="1">
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
       <c r="H159" s="7"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="6:8" ht="15.75" customHeight="1">
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
       <c r="H160" s="7"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="6:8" ht="15.75" customHeight="1">
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
       <c r="H161" s="7"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="6:8" ht="15.75" customHeight="1">
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
       <c r="H162" s="7"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="6:8" ht="15.75" customHeight="1">
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
       <c r="H163" s="7"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="6:8" ht="15.75" customHeight="1">
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
       <c r="H164" s="7"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="6:8" ht="15.75" customHeight="1">
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
       <c r="H165" s="7"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="6:8" ht="15.75" customHeight="1">
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
       <c r="H166" s="7"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="6:8" ht="15.75" customHeight="1">
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
       <c r="H167" s="7"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="6:8" ht="15.75" customHeight="1">
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
       <c r="H168" s="7"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="6:8" ht="15.75" customHeight="1">
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
       <c r="H169" s="7"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="6:8" ht="15.75" customHeight="1">
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
       <c r="H170" s="7"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="6:8" ht="15.75" customHeight="1">
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
       <c r="H171" s="7"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="6:8" ht="15.75" customHeight="1">
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
       <c r="H172" s="7"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="6:8" ht="15.75" customHeight="1">
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
       <c r="H173" s="7"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="6:8" ht="15.75" customHeight="1">
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
       <c r="H174" s="7"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="6:8" ht="15.75" customHeight="1">
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
       <c r="H175" s="7"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="6:8" ht="15.75" customHeight="1">
       <c r="F176" s="7"/>
       <c r="G176" s="7"/>
       <c r="H176" s="7"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="6:8" ht="15.75" customHeight="1">
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
       <c r="H177" s="7"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="6:8" ht="15.75" customHeight="1">
       <c r="F178" s="7"/>
       <c r="G178" s="7"/>
       <c r="H178" s="7"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="6:8" ht="15.75" customHeight="1">
       <c r="F179" s="7"/>
       <c r="G179" s="7"/>
       <c r="H179" s="7"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="6:8" ht="15.75" customHeight="1">
       <c r="F180" s="7"/>
       <c r="G180" s="7"/>
       <c r="H180" s="7"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="6:8" ht="15.75" customHeight="1">
       <c r="F181" s="7"/>
       <c r="G181" s="7"/>
       <c r="H181" s="7"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="6:8" ht="15.75" customHeight="1">
       <c r="F182" s="7"/>
       <c r="G182" s="7"/>
       <c r="H182" s="7"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="6:8" ht="15.75" customHeight="1">
       <c r="F183" s="7"/>
       <c r="G183" s="7"/>
       <c r="H183" s="7"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="6:8" ht="15.75" customHeight="1">
       <c r="F184" s="7"/>
       <c r="G184" s="7"/>
       <c r="H184" s="7"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="6:8" ht="15.75" customHeight="1">
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
       <c r="H185" s="7"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="6:8" ht="15.75" customHeight="1">
       <c r="F186" s="7"/>
       <c r="G186" s="7"/>
       <c r="H186" s="7"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="6:8" ht="15.75" customHeight="1">
       <c r="F187" s="7"/>
       <c r="G187" s="7"/>
       <c r="H187" s="7"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="6:8" ht="15.75" customHeight="1">
       <c r="F188" s="7"/>
       <c r="G188" s="7"/>
       <c r="H188" s="7"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="6:8" ht="15.75" customHeight="1">
       <c r="F189" s="7"/>
       <c r="G189" s="7"/>
       <c r="H189" s="7"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="6:8" ht="15.75" customHeight="1">
       <c r="F190" s="7"/>
       <c r="G190" s="7"/>
       <c r="H190" s="7"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="6:8" ht="15.75" customHeight="1">
       <c r="F191" s="7"/>
       <c r="G191" s="7"/>
       <c r="H191" s="7"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="6:8" ht="15.75" customHeight="1">
       <c r="F192" s="7"/>
       <c r="G192" s="7"/>
       <c r="H192" s="7"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="6:8" ht="15.75" customHeight="1">
       <c r="F193" s="7"/>
       <c r="G193" s="7"/>
       <c r="H193" s="7"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="6:8" ht="15.75" customHeight="1">
       <c r="F194" s="7"/>
       <c r="G194" s="7"/>
       <c r="H194" s="7"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="6:8" ht="15.75" customHeight="1">
       <c r="F195" s="7"/>
       <c r="G195" s="7"/>
       <c r="H195" s="7"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="6:8" ht="15.75" customHeight="1">
       <c r="F196" s="7"/>
       <c r="G196" s="7"/>
       <c r="H196" s="7"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="6:8" ht="15.75" customHeight="1">
       <c r="F197" s="7"/>
       <c r="G197" s="7"/>
       <c r="H197" s="7"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="6:8" ht="15.75" customHeight="1">
       <c r="F198" s="7"/>
       <c r="G198" s="7"/>
       <c r="H198" s="7"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="6:8" ht="15.75" customHeight="1">
       <c r="F199" s="7"/>
       <c r="G199" s="7"/>
       <c r="H199" s="7"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="6:8" ht="15.75" customHeight="1">
       <c r="F200" s="7"/>
       <c r="G200" s="7"/>
       <c r="H200" s="7"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="6:8" ht="15.75" customHeight="1">
       <c r="F201" s="7"/>
       <c r="G201" s="7"/>
       <c r="H201" s="7"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="6:8" ht="15.75" customHeight="1">
       <c r="F202" s="7"/>
       <c r="G202" s="7"/>
       <c r="H202" s="7"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="6:8" ht="15.75" customHeight="1">
       <c r="F203" s="7"/>
       <c r="G203" s="7"/>
       <c r="H203" s="7"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="6:8" ht="15.75" customHeight="1">
       <c r="F204" s="7"/>
       <c r="G204" s="7"/>
       <c r="H204" s="7"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="6:8" ht="15.75" customHeight="1">
       <c r="F205" s="7"/>
       <c r="G205" s="7"/>
       <c r="H205" s="7"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="6:8" ht="15.75" customHeight="1">
       <c r="F206" s="7"/>
       <c r="G206" s="7"/>
       <c r="H206" s="7"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="6:8" ht="15.75" customHeight="1">
       <c r="F207" s="7"/>
       <c r="G207" s="7"/>
       <c r="H207" s="7"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="6:8" ht="15.75" customHeight="1">
       <c r="F208" s="7"/>
       <c r="G208" s="7"/>
       <c r="H208" s="7"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="6:8" ht="15.75" customHeight="1">
       <c r="F209" s="7"/>
       <c r="G209" s="7"/>
       <c r="H209" s="7"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="6:8" ht="15.75" customHeight="1">
       <c r="F210" s="7"/>
       <c r="G210" s="7"/>
       <c r="H210" s="7"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="6:8" ht="15.75" customHeight="1">
       <c r="F211" s="7"/>
       <c r="G211" s="7"/>
       <c r="H211" s="7"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="6:8" ht="15.75" customHeight="1">
       <c r="F212" s="7"/>
       <c r="G212" s="7"/>
       <c r="H212" s="7"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="6:8" ht="15.75" customHeight="1">
       <c r="F213" s="7"/>
       <c r="G213" s="7"/>
       <c r="H213" s="7"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="6:8" ht="15.75" customHeight="1">
       <c r="F214" s="7"/>
       <c r="G214" s="7"/>
       <c r="H214" s="7"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="6:8" ht="15.75" customHeight="1">
       <c r="F215" s="7"/>
       <c r="G215" s="7"/>
       <c r="H215" s="7"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="6:8" ht="15.75" customHeight="1">
       <c r="F216" s="7"/>
       <c r="G216" s="7"/>
       <c r="H216" s="7"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="6:8" ht="15.75" customHeight="1">
       <c r="F217" s="7"/>
       <c r="G217" s="7"/>
       <c r="H217" s="7"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="6:8" ht="15.75" customHeight="1">
       <c r="F218" s="7"/>
       <c r="G218" s="7"/>
       <c r="H218" s="7"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="6:8" ht="15.75" customHeight="1">
       <c r="F219" s="7"/>
       <c r="G219" s="7"/>
       <c r="H219" s="7"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="6:8" ht="15.75" customHeight="1">
       <c r="F220" s="7"/>
       <c r="G220" s="7"/>
       <c r="H220" s="7"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
+    <row r="221" spans="6:8" ht="15.75" customHeight="1">
       <c r="F221" s="7"/>
       <c r="G221" s="7"/>
       <c r="H221" s="7"/>
     </row>
-    <row r="222" ht="15.75" customHeight="1">
+    <row r="222" spans="6:8" ht="15.75" customHeight="1">
       <c r="F222" s="7"/>
       <c r="G222" s="7"/>
       <c r="H222" s="7"/>
     </row>
-    <row r="223" ht="15.75" customHeight="1">
+    <row r="223" spans="6:8" ht="15.75" customHeight="1">
       <c r="F223" s="7"/>
       <c r="G223" s="7"/>
       <c r="H223" s="7"/>
     </row>
-    <row r="224" ht="15.75" customHeight="1">
+    <row r="224" spans="6:8" ht="15.75" customHeight="1">
       <c r="F224" s="7"/>
       <c r="G224" s="7"/>
       <c r="H224" s="7"/>
     </row>
-    <row r="225" ht="15.75" customHeight="1">
+    <row r="225" spans="6:8" ht="15.75" customHeight="1">
       <c r="F225" s="7"/>
       <c r="G225" s="7"/>
       <c r="H225" s="7"/>
     </row>
-    <row r="226" ht="15.75" customHeight="1">
+    <row r="226" spans="6:8" ht="15.75" customHeight="1">
       <c r="F226" s="7"/>
       <c r="G226" s="7"/>
       <c r="H226" s="7"/>
     </row>
-    <row r="227" ht="15.75" customHeight="1">
+    <row r="227" spans="6:8" ht="15.75" customHeight="1">
       <c r="F227" s="7"/>
       <c r="G227" s="7"/>
       <c r="H227" s="7"/>
     </row>
-    <row r="228" ht="15.75" customHeight="1">
+    <row r="228" spans="6:8" ht="15.75" customHeight="1">
       <c r="F228" s="7"/>
       <c r="G228" s="7"/>
       <c r="H228" s="7"/>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
+    <row r="229" spans="6:8" ht="15.75" customHeight="1">
       <c r="F229" s="7"/>
       <c r="G229" s="7"/>
       <c r="H229" s="7"/>
     </row>
-    <row r="230" ht="15.75" customHeight="1">
+    <row r="230" spans="6:8" ht="15.75" customHeight="1">
       <c r="F230" s="7"/>
       <c r="G230" s="7"/>
       <c r="H230" s="7"/>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" spans="6:8" ht="15.75" customHeight="1">
       <c r="F231" s="7"/>
       <c r="G231" s="7"/>
       <c r="H231" s="7"/>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
+    <row r="232" spans="6:8" ht="15.75" customHeight="1">
       <c r="F232" s="7"/>
       <c r="G232" s="7"/>
       <c r="H232" s="7"/>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" spans="6:8" ht="15.75" customHeight="1">
       <c r="F233" s="7"/>
       <c r="G233" s="7"/>
       <c r="H233" s="7"/>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" spans="6:8" ht="15.75" customHeight="1">
       <c r="F234" s="7"/>
       <c r="G234" s="7"/>
       <c r="H234" s="7"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
+    <row r="235" spans="6:8" ht="15.75" customHeight="1">
       <c r="F235" s="7"/>
       <c r="G235" s="7"/>
       <c r="H235" s="7"/>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" spans="6:8" ht="15.75" customHeight="1">
       <c r="F236" s="7"/>
       <c r="G236" s="7"/>
       <c r="H236" s="7"/>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" spans="6:8" ht="15.75" customHeight="1">
       <c r="F237" s="7"/>
       <c r="G237" s="7"/>
       <c r="H237" s="7"/>
     </row>
-    <row r="238" ht="15.75" customHeight="1">
+    <row r="238" spans="6:8" ht="15.75" customHeight="1">
       <c r="F238" s="7"/>
       <c r="G238" s="7"/>
       <c r="H238" s="7"/>
     </row>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="239" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="240" spans="6:8" ht="15.75" customHeight="1"/>
     <row r="241" ht="15.75" customHeight="1"/>
     <row r="242" ht="15.75" customHeight="1"/>
     <row r="243" ht="15.75" customHeight="1"/>
@@ -4020,112 +4071,110 @@
     <mergeCell ref="I29:I31"/>
     <mergeCell ref="I36:I38"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="25.75"/>
-    <col customWidth="1" min="3" max="3" width="35.5"/>
-    <col customWidth="1" min="4" max="10" width="13.38"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" customWidth="1"/>
+    <col min="4" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1"/>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="B2" s="77"/>
-      <c r="C2" s="78"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="79" t="s">
+    <row r="1" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="2" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B3" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="80"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="81" t="s">
+      <c r="C3" s="92"/>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B4" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="75" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="83" t="s">
+    <row r="5" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B5" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="85"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="83" t="s">
+      <c r="D5" s="78"/>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B6" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="77" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="83" t="s">
+    <row r="7" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B7" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="79" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="83" t="s">
+    <row r="8" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B8" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="77" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="83" t="s">
+    <row r="9" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B9" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="77" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="83" t="s">
+    <row r="10" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B10" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="80" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="88" t="s">
+    <row r="11" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B11" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="89" t="s">
+      <c r="C11" s="82" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="C14" s="90"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="12" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="13" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="14" spans="2:4" ht="15.75" customHeight="1">
+      <c r="C14" s="83"/>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="16" spans="2:4" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -5114,9 +5163,7 @@
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>